<commit_message>
Acta de reunión / Actualización burndown
</commit_message>
<xml_diff>
--- a/scrum/planning/burndown.xlsx
+++ b/scrum/planning/burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jautu/github/iw/scrum/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB4F911-DF85-1742-9511-194982363C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE04B7A-DBCA-6047-9557-B42F04611C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="17540" activeTab="4" xr2:uid="{F778D463-D90C-C340-996D-4EE14E291D0A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29080" windowHeight="17540" activeTab="3" xr2:uid="{F778D463-D90C-C340-996D-4EE14E291D0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 8" sheetId="7" r:id="rId1"/>
@@ -1414,8 +1414,29 @@
             <c:numRef>
               <c:f>'Sprint 4'!$B$5:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.666666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6666666666666714</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3333333333333384</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1488,6 +1509,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1830,10 +1860,49 @@
             <c:numRef>
               <c:f>'Sprint 3'!$B$5:$B$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>16</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.07692307692308</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.15384615384616</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.230769230769237</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.307692307692314</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.38461538461539</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.461538461538467</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.538461538461544</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.61538461538462</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.692307692307697</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.7692307692307736</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8461538461538503</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9230769230769273</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1926,13 +1995,49 @@
             <c:numRef>
               <c:f>'Sprint 3'!$C$5:$C$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0" formatCode="0">
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7771,8 +7876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC34136-754B-DA47-9D95-DD0AF8B7EF81}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7805,40 +7910,75 @@
       <c r="A5" s="1">
         <v>44295</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3">
+        <v>26</v>
+      </c>
       <c r="E5">
         <f>B5/6</f>
-        <v>0</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44296</v>
       </c>
+      <c r="B6" s="4">
+        <f t="shared" ref="B6:B11" si="0">B5-$E$5</f>
+        <v>21.666666666666668</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44297</v>
       </c>
+      <c r="B7" s="4">
+        <f t="shared" si="0"/>
+        <v>17.333333333333336</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44298</v>
       </c>
+      <c r="B8" s="4">
+        <f t="shared" si="0"/>
+        <v>13.000000000000004</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44299</v>
       </c>
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>8.6666666666666714</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44300</v>
       </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.3333333333333384</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44301</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -7854,8 +7994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55106EC1-B75D-7344-B2CA-B59BD49FD08B}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7889,82 +8029,170 @@
         <v>44281</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E5">
-        <f>B5/6</f>
-        <v>2.6666666666666665</v>
+        <f>B5/13</f>
+        <v>2.9230769230769229</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44282</v>
       </c>
+      <c r="B6" s="4">
+        <f>B5-$E$5</f>
+        <v>35.07692307692308</v>
+      </c>
+      <c r="C6" s="4">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44283</v>
       </c>
+      <c r="B7" s="4">
+        <f t="shared" ref="B7:B18" si="0">B6-$E$5</f>
+        <v>32.15384615384616</v>
+      </c>
+      <c r="C7" s="4">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44284</v>
       </c>
+      <c r="B8" s="4">
+        <f t="shared" si="0"/>
+        <v>29.230769230769237</v>
+      </c>
       <c r="C8">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44285</v>
       </c>
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>26.307692307692314</v>
+      </c>
+      <c r="C9" s="4">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44286</v>
       </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>23.38461538461539</v>
+      </c>
+      <c r="C10" s="4">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44287</v>
       </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>20.461538461538467</v>
+      </c>
+      <c r="C11" s="4">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44288</v>
       </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>17.538461538461544</v>
+      </c>
+      <c r="C12" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44289</v>
       </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>14.61538461538462</v>
+      </c>
+      <c r="C13" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44290</v>
       </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>11.692307692307697</v>
+      </c>
+      <c r="C14" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44291</v>
       </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>8.7692307692307736</v>
+      </c>
+      <c r="C15" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44292</v>
       </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>5.8461538461538503</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44293</v>
       </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9230769230769273</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44294</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4408920985006262E-15</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7978,7 +8206,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8105,7 +8333,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Ampliada la documentación de p2
</commit_message>
<xml_diff>
--- a/scrum/planning/burndown.xlsx
+++ b/scrum/planning/burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jautu/github/iw/scrum/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE04B7A-DBCA-6047-9557-B42F04611C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2027058-B379-8744-B0E3-17D152F27947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29080" windowHeight="17540" activeTab="3" xr2:uid="{F778D463-D90C-C340-996D-4EE14E291D0A}"/>
   </bookViews>
@@ -1417,22 +1417,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.666666666666668</c:v>
+                  <c:v>23.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.333333333333336</c:v>
+                  <c:v>18.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.000000000000004</c:v>
+                  <c:v>13.999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6666666666666714</c:v>
+                  <c:v>9.3333333333333286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3333333333333384</c:v>
+                  <c:v>4.6666666666666616</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1510,10 +1510,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="0.00">
-                  <c:v>26</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
@@ -7877,7 +7877,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7911,14 +7911,14 @@
         <v>44295</v>
       </c>
       <c r="B5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <f>B5/6</f>
-        <v>4.333333333333333</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -7927,10 +7927,10 @@
       </c>
       <c r="B6" s="4">
         <f t="shared" ref="B6:B11" si="0">B5-$E$5</f>
-        <v>21.666666666666668</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -7939,7 +7939,7 @@
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
-        <v>17.333333333333336</v>
+        <v>18.666666666666664</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -7951,7 +7951,7 @@
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
-        <v>13.000000000000004</v>
+        <v>13.999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -7960,7 +7960,7 @@
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
-        <v>8.6666666666666714</v>
+        <v>9.3333333333333286</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -7969,7 +7969,7 @@
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
-        <v>4.3333333333333384</v>
+        <v>4.6666666666666616</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>